<commit_message>
working correlation in returned csv
</commit_message>
<xml_diff>
--- a/pr_120_vs_creativity.xlsx
+++ b/pr_120_vs_creativity.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26915"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Varun/Google Drive/Research/Spring 2016/network-creativity/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="340" yWindow="-16320" windowWidth="23920" windowHeight="15780" tabRatio="500"/>
+    <workbookView xWindow="340" yWindow="460" windowWidth="23920" windowHeight="15780" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="pr_120.csv" sheetId="1" r:id="rId1"/>
@@ -15,8 +20,11 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">pr_120.csv!$A$2:$G$2</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -1533,11 +1541,16 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="timing_ideas_with_ratings.csv"/>
@@ -21411,9 +21424,9 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="H1">
         <f>CORREL($F3:$F122,H3:H122)</f>
         <v>-0.10229055941032024</v>
@@ -21427,7 +21440,7 @@
         <v>-0.14183288564134366</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -21456,7 +21469,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>97</v>
       </c>
@@ -21473,7 +21486,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>62</v>
       </c>
@@ -21508,7 +21521,7 @@
         <v>2.046740993083787</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>81</v>
       </c>
@@ -21543,7 +21556,7 @@
         <v>3.5122248348271143</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -21578,7 +21591,7 @@
         <v>1.6346721548373155</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -21613,7 +21626,7 @@
         <v>0.54043410413311477</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -21648,7 +21661,7 @@
         <v>2.5994300878771583</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>9</v>
       </c>
@@ -21683,7 +21696,7 @@
         <v>3.2543074381599091</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>10</v>
       </c>
@@ -21718,7 +21731,7 @@
         <v>7.914271935518963</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>11</v>
       </c>
@@ -21753,7 +21766,7 @@
         <v>3.4254937197460111</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>13</v>
       </c>
@@ -21788,7 +21801,7 @@
         <v>3.749395108003847</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>17</v>
       </c>
@@ -21823,7 +21836,7 @@
         <v>3.4462874957649863</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>18</v>
       </c>
@@ -21858,7 +21871,7 @@
         <v>1.7310199541680715</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>19</v>
       </c>
@@ -21893,7 +21906,7 @@
         <v>1.5865419603652835</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>20</v>
       </c>
@@ -21928,7 +21941,7 @@
         <v>2.0454326618039</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>21</v>
       </c>
@@ -21963,7 +21976,7 @@
         <v>4.0466246476053334</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>22</v>
       </c>
@@ -21998,7 +22011,7 @@
         <v>4.9526783642673289</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>23</v>
       </c>
@@ -22033,7 +22046,7 @@
         <v>3.1170076215929137</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>26</v>
       </c>
@@ -22068,7 +22081,7 @@
         <v>4.1272867837562668</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>29</v>
       </c>
@@ -22103,7 +22116,7 @@
         <v>1.0823434621032093</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>33</v>
       </c>
@@ -22138,7 +22151,7 @@
         <v>3.6360869332309025</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>34</v>
       </c>
@@ -22173,7 +22186,7 @@
         <v>0.88784800442791445</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>35</v>
       </c>
@@ -22208,7 +22221,7 @@
         <v>4.4851458732209029</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>38</v>
       </c>
@@ -22243,7 +22256,7 @@
         <v>3.892471644189734</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>39</v>
       </c>
@@ -22278,7 +22291,7 @@
         <v>4.341753009772364</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>40</v>
       </c>
@@ -22313,7 +22326,7 @@
         <v>1.2585982997479546</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>46</v>
       </c>
@@ -22348,7 +22361,7 @@
         <v>2.0818553510283389</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>48</v>
       </c>
@@ -22383,7 +22396,7 @@
         <v>2.4435130806251242</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>50</v>
       </c>
@@ -22418,7 +22431,7 @@
         <v>5.6792032027306627</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>52</v>
       </c>
@@ -22453,7 +22466,7 @@
         <v>7.8095446465779528</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>54</v>
       </c>
@@ -22488,7 +22501,7 @@
         <v>6.0484411396153748</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>55</v>
       </c>
@@ -22523,7 +22536,7 @@
         <v>4.0754705515286345</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>56</v>
       </c>
@@ -22558,7 +22571,7 @@
         <v>2.7348884075306721</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>58</v>
       </c>
@@ -22593,7 +22606,7 @@
         <v>3.6434951730050749</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>59</v>
       </c>
@@ -22628,7 +22641,7 @@
         <v>3.4923714977142857</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>61</v>
       </c>
@@ -22663,7 +22676,7 @@
         <v>3.1148509059643943</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>63</v>
       </c>
@@ -22698,7 +22711,7 @@
         <v>0.76429984264349804</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>66</v>
       </c>
@@ -22733,7 +22746,7 @@
         <v>2.8479408170894729</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>67</v>
       </c>
@@ -22768,7 +22781,7 @@
         <v>4.8479654879671301</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>68</v>
       </c>
@@ -22803,7 +22816,7 @@
         <v>1.4369908612859355</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>71</v>
       </c>
@@ -22838,7 +22851,7 @@
         <v>2.0707632771362863</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>72</v>
       </c>
@@ -22873,7 +22886,7 @@
         <v>2.4387482024731506</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>73</v>
       </c>
@@ -22908,7 +22921,7 @@
         <v>1.9372858438267473</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>78</v>
       </c>
@@ -22943,7 +22956,7 @@
         <v>1.9131303746334023</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>79</v>
       </c>
@@ -22978,7 +22991,7 @@
         <v>4.5267072897033707</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>80</v>
       </c>
@@ -23013,7 +23026,7 @@
         <v>1.0072641861628993</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>83</v>
       </c>
@@ -23048,7 +23061,7 @@
         <v>6.5724233386072699</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>84</v>
       </c>
@@ -23083,7 +23096,7 @@
         <v>0.16571612643585748</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>87</v>
       </c>
@@ -23118,7 +23131,7 @@
         <v>2.8946919961676962</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>88</v>
       </c>
@@ -23153,7 +23166,7 @@
         <v>2.9326913351806265</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>89</v>
       </c>
@@ -23188,7 +23201,7 @@
         <v>1.1517196188949088</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>95</v>
       </c>
@@ -23223,7 +23236,7 @@
         <v>4.1950835690079806</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>96</v>
       </c>
@@ -23258,7 +23271,7 @@
         <v>1.768717170673018</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>98</v>
       </c>
@@ -23293,7 +23306,7 @@
         <v>1.062182396072648</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>100</v>
       </c>
@@ -23328,7 +23341,7 @@
         <v>2.4372404379070196</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>103</v>
       </c>
@@ -23363,7 +23376,7 @@
         <v>2.2505081047664448</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>108</v>
       </c>
@@ -23398,7 +23411,7 @@
         <v>5.7453760265524476</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>111</v>
       </c>
@@ -23433,7 +23446,7 @@
         <v>0.74242983374151073</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>112</v>
       </c>
@@ -23468,7 +23481,7 @@
         <v>2.5349053936312749</v>
       </c>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>113</v>
       </c>
@@ -23503,7 +23516,7 @@
         <v>3.1680726350335449</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>115</v>
       </c>
@@ -23538,7 +23551,7 @@
         <v>4.6528913206064413</v>
       </c>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>117</v>
       </c>
@@ -23573,7 +23586,7 @@
         <v>3.3464176771567757</v>
       </c>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>119</v>
       </c>
@@ -23608,7 +23621,7 @@
         <v>2.0169298849967312</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>12</v>
       </c>
@@ -23643,7 +23656,7 @@
         <v>4.8543702874404833</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>25</v>
       </c>
@@ -23678,7 +23691,7 @@
         <v>3.1685307450931872</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>27</v>
       </c>
@@ -23713,7 +23726,7 @@
         <v>2.665997787651007</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>51</v>
       </c>
@@ -23748,7 +23761,7 @@
         <v>4.0252857965602056</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>64</v>
       </c>
@@ -23783,7 +23796,7 @@
         <v>4.6422971803822088</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>70</v>
       </c>
@@ -23818,7 +23831,7 @@
         <v>2.2087538766470711</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>85</v>
       </c>
@@ -23853,7 +23866,7 @@
         <v>1.5830228283865446</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>0</v>
       </c>
@@ -23888,7 +23901,7 @@
         <v>4.3751172140875099</v>
       </c>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>3</v>
       </c>
@@ -23923,7 +23936,7 @@
         <v>3.8462114907776201</v>
       </c>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>5</v>
       </c>
@@ -23958,7 +23971,7 @@
         <v>4.0327951072189885</v>
       </c>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>8</v>
       </c>
@@ -23993,7 +24006,7 @@
         <v>2.2821535484367597</v>
       </c>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>14</v>
       </c>
@@ -24028,7 +24041,7 @@
         <v>2.1157082093503288</v>
       </c>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>15</v>
       </c>
@@ -24063,7 +24076,7 @@
         <v>0.53649821561893718</v>
       </c>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>16</v>
       </c>
@@ -24098,7 +24111,7 @@
         <v>0.4337143572263179</v>
       </c>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>24</v>
       </c>
@@ -24133,7 +24146,7 @@
         <v>3.3068322365465415</v>
       </c>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>28</v>
       </c>
@@ -24168,7 +24181,7 @@
         <v>1.7284138315321089</v>
       </c>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>30</v>
       </c>
@@ -24203,7 +24216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>31</v>
       </c>
@@ -24238,7 +24251,7 @@
         <v>1.6144144145237762</v>
       </c>
     </row>
-    <row r="83" spans="1:10">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>32</v>
       </c>
@@ -24273,7 +24286,7 @@
         <v>2.8095049250509838</v>
       </c>
     </row>
-    <row r="84" spans="1:10">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>36</v>
       </c>
@@ -24308,7 +24321,7 @@
         <v>0.61751955199250108</v>
       </c>
     </row>
-    <row r="85" spans="1:10">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>37</v>
       </c>
@@ -24343,7 +24356,7 @@
         <v>2.6856178931558334</v>
       </c>
     </row>
-    <row r="86" spans="1:10">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>45</v>
       </c>
@@ -24378,7 +24391,7 @@
         <v>3.3988452007248959</v>
       </c>
     </row>
-    <row r="87" spans="1:10">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>47</v>
       </c>
@@ -24413,7 +24426,7 @@
         <v>3.7076535283045717</v>
       </c>
     </row>
-    <row r="88" spans="1:10">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>53</v>
       </c>
@@ -24448,7 +24461,7 @@
         <v>7.5320503935998833</v>
       </c>
     </row>
-    <row r="89" spans="1:10">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>65</v>
       </c>
@@ -24483,7 +24496,7 @@
         <v>2.0630087374542425</v>
       </c>
     </row>
-    <row r="90" spans="1:10">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>74</v>
       </c>
@@ -24518,7 +24531,7 @@
         <v>2.2239285574813357</v>
       </c>
     </row>
-    <row r="91" spans="1:10">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>76</v>
       </c>
@@ -24553,7 +24566,7 @@
         <v>5.6160444524592696</v>
       </c>
     </row>
-    <row r="92" spans="1:10">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>77</v>
       </c>
@@ -24588,7 +24601,7 @@
         <v>2.1913239397627797</v>
       </c>
     </row>
-    <row r="93" spans="1:10">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>82</v>
       </c>
@@ -24623,7 +24636,7 @@
         <v>3.9607387080267022</v>
       </c>
     </row>
-    <row r="94" spans="1:10">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>90</v>
       </c>
@@ -24658,7 +24671,7 @@
         <v>4.0235698516300893</v>
       </c>
     </row>
-    <row r="95" spans="1:10">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>91</v>
       </c>
@@ -24693,7 +24706,7 @@
         <v>2.3210689337681085</v>
       </c>
     </row>
-    <row r="96" spans="1:10">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>93</v>
       </c>
@@ -24728,7 +24741,7 @@
         <v>3.5517614682954344</v>
       </c>
     </row>
-    <row r="97" spans="1:10">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>94</v>
       </c>
@@ -24763,7 +24776,7 @@
         <v>5.5647458254154632E-2</v>
       </c>
     </row>
-    <row r="98" spans="1:10">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>99</v>
       </c>
@@ -24798,7 +24811,7 @@
         <v>1.2351706870834895</v>
       </c>
     </row>
-    <row r="99" spans="1:10">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>102</v>
       </c>
@@ -24833,7 +24846,7 @@
         <v>1.0226137533142594</v>
       </c>
     </row>
-    <row r="100" spans="1:10">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>104</v>
       </c>
@@ -24868,7 +24881,7 @@
         <v>7.5374371346350095</v>
       </c>
     </row>
-    <row r="101" spans="1:10">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>106</v>
       </c>
@@ -24903,7 +24916,7 @@
         <v>3.6518434546505931</v>
       </c>
     </row>
-    <row r="102" spans="1:10">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>107</v>
       </c>
@@ -24938,7 +24951,7 @@
         <v>2.021697647066135</v>
       </c>
     </row>
-    <row r="103" spans="1:10">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>109</v>
       </c>
@@ -24973,7 +24986,7 @@
         <v>2.0789348838110184</v>
       </c>
     </row>
-    <row r="104" spans="1:10">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>110</v>
       </c>
@@ -25008,7 +25021,7 @@
         <v>2.0687950908824759</v>
       </c>
     </row>
-    <row r="105" spans="1:10">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>114</v>
       </c>
@@ -25043,7 +25056,7 @@
         <v>2.9029391800235032</v>
       </c>
     </row>
-    <row r="106" spans="1:10">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>116</v>
       </c>
@@ -25078,7 +25091,7 @@
         <v>1.9548060115701276</v>
       </c>
     </row>
-    <row r="107" spans="1:10">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>118</v>
       </c>
@@ -25113,7 +25126,7 @@
         <v>2.6075681146962744</v>
       </c>
     </row>
-    <row r="108" spans="1:10">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>1</v>
       </c>
@@ -25148,7 +25161,7 @@
         <v>6.0098249759677191</v>
       </c>
     </row>
-    <row r="109" spans="1:10">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>42</v>
       </c>
@@ -25183,7 +25196,7 @@
         <v>2.151697319636682</v>
       </c>
     </row>
-    <row r="110" spans="1:10">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>43</v>
       </c>
@@ -25218,7 +25231,7 @@
         <v>1.4114990501944946</v>
       </c>
     </row>
-    <row r="111" spans="1:10">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>44</v>
       </c>
@@ -25253,7 +25266,7 @@
         <v>0.50128467603756066</v>
       </c>
     </row>
-    <row r="112" spans="1:10">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>49</v>
       </c>
@@ -25288,7 +25301,7 @@
         <v>2.4060454635198463</v>
       </c>
     </row>
-    <row r="113" spans="1:10">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>57</v>
       </c>
@@ -25323,7 +25336,7 @@
         <v>3.0748835307998279</v>
       </c>
     </row>
-    <row r="114" spans="1:10">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>60</v>
       </c>
@@ -25358,7 +25371,7 @@
         <v>2.690421068490068</v>
       </c>
     </row>
-    <row r="115" spans="1:10">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>69</v>
       </c>
@@ -25393,7 +25406,7 @@
         <v>2.0972645700433907</v>
       </c>
     </row>
-    <row r="116" spans="1:10">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>75</v>
       </c>
@@ -25428,7 +25441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:10">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>86</v>
       </c>
@@ -25463,7 +25476,7 @@
         <v>4.0758799200848435</v>
       </c>
     </row>
-    <row r="118" spans="1:10">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>101</v>
       </c>
@@ -25498,7 +25511,7 @@
         <v>3.7319953304504327</v>
       </c>
     </row>
-    <row r="119" spans="1:10">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>105</v>
       </c>
@@ -25533,7 +25546,7 @@
         <v>2.1098798695599768</v>
       </c>
     </row>
-    <row r="120" spans="1:10">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>2</v>
       </c>
@@ -25568,7 +25581,7 @@
         <v>3.3468386946483375</v>
       </c>
     </row>
-    <row r="121" spans="1:10">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>41</v>
       </c>
@@ -25603,7 +25616,7 @@
         <v>1.595493202657648</v>
       </c>
     </row>
-    <row r="122" spans="1:10">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>92</v>
       </c>
@@ -25646,10 +25659,5 @@
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>